<commit_message>
AJUSTES CENTRAL DE MODELOS
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/REQUISICAO_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/REQUISICAO_MODELO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC Home\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126C71B6-3747-49B8-9985-3215934EDD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA4065B-5687-424D-AEE6-B520ACA9191E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{795787B9-A603-4E9F-9555-87E07481D83A}"/>
   </bookViews>
@@ -209,57 +209,57 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,7 +578,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,127 +589,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="13"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="9" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="13"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="7" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="14" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EMISSÃO DE ORDEM DE SERVIÇO
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/REQUISICAO_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/REQUISICAO_MODELO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B296FEA-AEC0-404C-9729-8D28BC8B1A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F870E46F-3426-49D8-AEF7-BD5B12CAD0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{795787B9-A603-4E9F-9555-87E07481D83A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>N. REQUISIÇÃO</t>
   </si>
@@ -81,13 +81,16 @@
   </si>
   <si>
     <t>OBSERVAÇÃO</t>
+  </si>
+  <si>
+    <t>PDDC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +114,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,7 +138,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -160,19 +178,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -206,63 +211,124 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC889DE-7B05-4795-BCD8-9882F919D78A}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,151 +660,540 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="14" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="13"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="14" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="15" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="15"/>
-      <c r="M4" s="2"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="14" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="13"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="13"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="3" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="M8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="6"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C5:D5"/>
+  <mergeCells count="23">
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="F6:N6"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="G3:N3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E8:L8"/>
+    <mergeCell ref="F8:K8"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G3:M3"/>
     <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="F6:M6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E3:F3"/>
@@ -746,8 +1201,10 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
-  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Negrito"&amp;14RELATÓRIO DE REQUISIÇÃO DE MATERIAL</oddHeader>

</xml_diff>

<commit_message>
AJUSTES REQUISIÇÃO, CANCELA SOLICITAÇÃO O.S SELEÇÃO DE CAMINHO PARA RE-IMPRIMIR
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/REQUISICAO_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/REQUISICAO_MODELO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627EE767-B991-429B-85A0-0E8293900234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5710095-3D83-4EDF-AE7A-5BB2B4951CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{795787B9-A603-4E9F-9555-87E07481D83A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{795787B9-A603-4E9F-9555-87E07481D83A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>N. REQUISIÇÃO</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>RELATÓRIO DE REQUISIÇÃO DE MATERIAL</t>
+  </si>
+  <si>
+    <t>VOLUME</t>
   </si>
 </sst>
 </file>
@@ -144,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -215,15 +218,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -278,10 +272,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -291,22 +309,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -316,30 +334,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -659,7 +653,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,116 +662,132 @@
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="11" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="13" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="24"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="11" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="22"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="22"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -786,421 +796,416 @@
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
       <c r="L8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="19"/>
-      <c r="O8" s="3"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="G3:N3"/>
-    <mergeCell ref="E8:K8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="F6:N6"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="M4:N4"/>
+  <mergeCells count="24">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
@@ -1217,9 +1222,17 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="G3:N3"/>
+    <mergeCell ref="E8:K8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="F6:N6"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="A7:N7"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;"-,Negrito"Impresso em:  &amp;D</oddFooter>
   </headerFooter>

</xml_diff>